<commit_message>
Clean up DynamicArrays project
</commit_message>
<xml_diff>
--- a/SpecialTopics/DynamicArrays/Examples.xlsx
+++ b/SpecialTopics/DynamicArrays/Examples.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Excel-DNA\Tutorials\SpecialTopics\DynamicArrays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FD6F99-FB22-4647-9CCC-31A8A04C2A36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F33C421-7725-405F-870F-9CB167B28B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{1310C58F-A79A-4977-8141-61E3ED8E730D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1310C58F-A79A-4977-8141-61E3ED8E730D}"/>
   </bookViews>
   <sheets>
     <sheet name="ArrayResult" sheetId="3" r:id="rId1"/>
     <sheet name="ArrayInput" sheetId="4" r:id="rId2"/>
     <sheet name="NormalFunction" sheetId="5" r:id="rId3"/>
-    <sheet name="ImplicitIntersectionAndResize" sheetId="2" r:id="rId4"/>
+    <sheet name="ImplicitIntersection" sheetId="2" r:id="rId4"/>
     <sheet name="ArrayReference" sheetId="8" r:id="rId5"/>
     <sheet name="ArrayMap" sheetId="7" r:id="rId6"/>
     <sheet name="ArrayAsync" sheetId="1" r:id="rId7"/>
-    <sheet name="ArrayResizer" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>dnaMakeArray</t>
   </si>
@@ -128,34 +127,25 @@
     <t>Supports DA</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>dnaArrayMap</t>
   </si>
   <si>
     <t>dnaDescribe(dnaArrayGetHead)</t>
   </si>
   <si>
-    <t>dnaResize()</t>
+    <t>dnaDescribeArray</t>
+  </si>
+  <si>
+    <t>dnaAddPrefix</t>
+  </si>
+  <si>
+    <t>Delay(ms)</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>dnaMakeArrayAsync</t>
   </si>
 </sst>
 </file>
@@ -517,50 +507,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB45A32-B4A5-4781-B2AA-A61A53D7C8D2}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D817620D-9222-4C08-8764-35A36318E92A}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="K4" sqref="K4:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,157 +554,54 @@
     <col min="9" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="B4" cm="1">
+        <f t="array" ref="B4:D5">_xlfn.SEQUENCE(B1,B2)</f>
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="L4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M5" cm="1">
-        <f t="array" ref="M5:O5">_xlfn.SEQUENCE(,$L$4)</f>
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" cm="1">
-        <f t="array" ref="B6:D7">_xlfn.SEQUENCE(B3,B4)</f>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="str" cm="1">
-        <f t="array" ref="H6:H13">CHAR(64+_xlfn.SEQUENCE($I$4))</f>
-        <v>A</v>
-      </c>
-      <c r="I6" cm="1">
-        <f t="array" ref="I6:I13">_xlfn.SEQUENCE(I4)</f>
-        <v>1</v>
-      </c>
-      <c r="L6" t="str" cm="1">
-        <f t="array" ref="L6:L8">CHAR(64+_xlfn.SEQUENCE($L$4))</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C5">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="D5">
         <v>6</v>
-      </c>
-      <c r="H7" t="str">
-        <v>B</v>
-      </c>
-      <c r="I7">
-        <v>2</v>
-      </c>
-      <c r="L7" t="str">
-        <v>B</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H8" t="str">
-        <v>C</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="L8" t="str">
-        <v>C</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H9" t="str">
-        <v>D</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H10" t="str">
-        <v>E</v>
-      </c>
-      <c r="I10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H11" t="str">
-        <v>F</v>
-      </c>
-      <c r="I11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H12" t="str">
-        <v>G</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="H13" t="str">
-        <v>H</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -733,10 +612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEA9CC6-A58B-4F7F-8C44-9CBD90AD5FFC}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,41 +625,32 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
-        <v>2</v>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
+      <c r="A6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -794,7 +664,7 @@
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,9 +676,9 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
+      <c r="B1" t="b" cm="1">
+        <f t="array" ref="B1">_xll.dnaSupportsDynamicArrays()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -877,23 +747,23 @@
       <c r="A7">
         <v>2</v>
       </c>
-      <c r="C7" t="e" cm="1">
-        <f t="array" aca="1" ref="C7" ca="1">_xll.dnaAddThem(_xlfn.ANCHORARRAY($A$6),_xlfn.ANCHORARRAY( $B$5))</f>
-        <v>#NAME?</v>
+      <c r="C7" cm="1">
+        <f t="array" ref="C7">_xll.dnaAddThem(_xlfn.ANCHORARRAY($A$6),_xlfn.ANCHORARRAY( $B$5))</f>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="H7" t="e">
-        <f ca="1">_xll.dnaAddThem(_xlfn.ANCHORARRAY($F$6),_xlfn.ANCHORARRAY( $G$5))</f>
-        <v>#NAME?</v>
+      <c r="H7">
+        <f>_xll.dnaAddThem(_xlfn.ANCHORARRAY($F$6),_xlfn.ANCHORARRAY( $G$5))</f>
+        <v>14</v>
       </c>
       <c r="K7">
         <v>2</v>
       </c>
-      <c r="M7" t="e">
-        <f t="array" aca="1" ref="M7" ca="1">_xll.dnaAddThem(_xlfn.ANCHORARRAY($K$6),_xlfn.ANCHORARRAY( $L$5))</f>
-        <v>#NAME?</v>
+      <c r="M7">
+        <f t="array" ref="M7">_xll.dnaAddThem(_xlfn.ANCHORARRAY($K$6),_xlfn.ANCHORARRAY( $L$5))</f>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -980,25 +850,29 @@
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="e" cm="1">
-        <f t="array" aca="1" ref="B13" ca="1">dnaConcatenate($A$13:$A16,_xlfn.ANCHORARRAY($B$12))</f>
-        <v>#NAME?</v>
+      <c r="B13" t="str" cm="1">
+        <f t="array" ref="B13:D13">_xll.dnaConcatenate($A$13:$A16,_xlfn.ANCHORARRAY($B$12))</f>
+        <v>111ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="C13" t="str">
+        <v>121ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="D13" t="str">
+        <v>131ExcelDna.Integration.ExcelMissing</v>
       </c>
       <c r="F13" cm="1">
         <f t="array" ref="F13:F15">_xlfn.SEQUENCE(3)</f>
         <v>1</v>
       </c>
-      <c r="G13" t="e">
-        <f t="array" aca="1" ref="G13:I15" ca="1">dnaConcatenate(_xlfn.ANCHORARRAY($F$13),_xlfn.ANCHORARRAY($G$12))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="G13" t="str">
+        <f t="array" ref="G13:I15">_xll.dnaConcatenate(_xlfn.ANCHORARRAY($F$13),_xlfn.ANCHORARRAY($G$12))</f>
+        <v>111ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="H13" t="str">
+        <v>121ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="I13" t="str">
+        <v>131ExcelDna.Integration.ExcelMissing</v>
       </c>
       <c r="K13" cm="1">
         <f t="array" ref="K13:K16">_xlfn.SEQUENCE(4)</f>
@@ -1013,15 +887,7 @@
         <v>1</v>
       </c>
       <c r="Q13" t="e">
-        <f t="array" aca="1" ref="Q13:S15" ca="1">_xll.dnaResize(_xll.dnaAddThemDoubleArrays(_xlfn.ANCHORARRAY($P$13),_xlfn.ANCHORARRAY($Q$12)))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R13" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="S13" t="e">
-        <f ca="1"/>
+        <f t="array" aca="1" ref="Q13" ca="1">_xll.dnaResize(dnaAddThemDoubleArrays(_xlfn.ANCHORARRAY($P$13),_xlfn.ANCHORARRAY($Q$12)))</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -1032,70 +898,40 @@
       <c r="F14">
         <v>2</v>
       </c>
-      <c r="G14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="G14" t="str">
+        <v>111ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="H14" t="str">
+        <v>121ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="I14" t="str">
+        <v>131ExcelDna.Integration.ExcelMissing</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="P14">
         <v>2</v>
-      </c>
-      <c r="Q14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="R14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="S14" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>3</v>
       </c>
-      <c r="G15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
+      <c r="G15" t="str">
+        <v>111ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="H15" t="str">
+        <v>121ExcelDna.Integration.ExcelMissing</v>
+      </c>
+      <c r="I15" t="str">
+        <v>131ExcelDna.Integration.ExcelMissing</v>
       </c>
       <c r="K15">
         <v>3</v>
       </c>
       <c r="P15">
         <v>3</v>
-      </c>
-      <c r="Q15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="R15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="S15" t="e">
-        <f ca="1"/>
-        <v>#NAME?</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1129,9 +965,9 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
+      <c r="B1" t="b" cm="1">
+        <f t="array" ref="B1">_xll.dnaSupportsDynamicArrays()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1145,13 +981,13 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="K5" t="e" cm="1">
-        <f t="array" aca="1" ref="K5" ca="1">_xll.dnaArrayGetHead(_xlfn.ANCHORARRAY(#REF!), 4)</f>
-        <v>#NAME?</v>
+        <f t="array" ref="K5">_xll.dnaArrayGetHead(_xlfn.ANCHORARRAY(#REF!), 4)</f>
+        <v>#REF!</v>
       </c>
       <c r="P5" t="e" cm="1">
         <f t="array" aca="1" ref="P5" ca="1">_xll.dnaDescribe(_xlfn.ANCHORARRAY(K5))</f>
@@ -1169,10 +1005,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54127A86-56AF-42BB-8D1B-18B2F8870479}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,18 +1016,50 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="b" cm="1">
+        <f t="array" ref="B1">_xll.dnaSupportsDynamicArrays()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1201,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503EA15C-7DA0-4BE1-B06C-0B273AE21457}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,102 +1081,97 @@
     <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="e" cm="1">
-        <f t="array" aca="1" ref="A3" ca="1">_xll.dnaMakeArrayAsync(3000,4,5)</f>
-        <v>#NAME?</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="str" cm="1">
+        <f t="array" ref="A6:E9">_xll.dnaMakeArrayAsync(3000,4,5)</f>
+        <v>0|0</v>
+      </c>
+      <c r="B6" t="str">
+        <v>0|1</v>
+      </c>
+      <c r="C6" t="str">
+        <v>0|2</v>
+      </c>
+      <c r="D6" t="str">
+        <v>0|3</v>
+      </c>
+      <c r="E6" t="str">
+        <v>0|4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <v>1|0</v>
+      </c>
+      <c r="B7" t="str">
+        <v>1|1</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1|2</v>
+      </c>
+      <c r="D7" t="str">
+        <v>1|3</v>
+      </c>
+      <c r="E7" t="str">
+        <v>1|4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <v>2|0</v>
+      </c>
+      <c r="B8" t="str">
+        <v>2|1</v>
+      </c>
+      <c r="C8" t="str">
+        <v>2|2</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2|3</v>
+      </c>
+      <c r="E8" t="str">
+        <v>2|4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <v>3|0</v>
+      </c>
+      <c r="B9" t="str">
+        <v>3|1</v>
+      </c>
+      <c r="C9" t="str">
+        <v>3|2</v>
+      </c>
+      <c r="D9" t="str">
+        <v>3|3</v>
+      </c>
+      <c r="E9" t="str">
+        <v>3|4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B138100F-09C0-4DA4-8158-824EE415D812}">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="e" cm="1">
-        <f t="array" aca="1" ref="B1" ca="1">dnaSupportsDynamicArrays()</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>